<commit_message>
food page 구현 완료
</commit_message>
<xml_diff>
--- a/data/FoodData.xlsx
+++ b/data/FoodData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1447" uniqueCount="684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="685">
   <si>
     <t>FOODID</t>
   </si>
@@ -757,7 +757,7 @@
     <t>SP0001</t>
   </si>
   <si>
-    <t>SP0002</t>
+    <t>T0001</t>
   </si>
   <si>
     <t>CAMBODIA</t>
@@ -1424,6 +1424,9 @@
   </si>
   <si>
     <t>Caramelized Pork with Eggs</t>
+  </si>
+  <si>
+    <t>test food</t>
   </si>
   <si>
     <t>R00171</t>
@@ -2423,7 +2426,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB238"/>
+  <dimension ref="A1:AB232"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2529,7 +2532,7 @@
         <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="F2" t="s">
         <v>252</v>
@@ -2609,7 +2612,7 @@
         <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="F3" t="s">
         <v>253</v>
@@ -2689,7 +2692,7 @@
         <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="F4" t="s">
         <v>254</v>
@@ -2769,7 +2772,7 @@
         <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="F5" t="s">
         <v>255</v>
@@ -2849,7 +2852,7 @@
         <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="F6" t="s">
         <v>256</v>
@@ -2929,7 +2932,7 @@
         <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="F7" t="s">
         <v>257</v>
@@ -3009,7 +3012,7 @@
         <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="F8" t="s">
         <v>258</v>
@@ -3089,7 +3092,7 @@
         <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="F9" t="s">
         <v>259</v>
@@ -3169,7 +3172,7 @@
         <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F10" t="s">
         <v>260</v>
@@ -3249,7 +3252,7 @@
         <v>37</v>
       </c>
       <c r="E11" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="F11" t="s">
         <v>261</v>
@@ -3329,7 +3332,7 @@
         <v>38</v>
       </c>
       <c r="E12" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="F12" t="s">
         <v>262</v>
@@ -3409,7 +3412,7 @@
         <v>39</v>
       </c>
       <c r="E13" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="F13" t="s">
         <v>263</v>
@@ -3489,7 +3492,7 @@
         <v>40</v>
       </c>
       <c r="E14" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="F14" t="s">
         <v>264</v>
@@ -3569,7 +3572,7 @@
         <v>41</v>
       </c>
       <c r="E15" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="F15" t="s">
         <v>265</v>
@@ -3649,7 +3652,7 @@
         <v>42</v>
       </c>
       <c r="E16" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="F16" t="s">
         <v>266</v>
@@ -3729,7 +3732,7 @@
         <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="F17" t="s">
         <v>267</v>
@@ -3809,7 +3812,7 @@
         <v>44</v>
       </c>
       <c r="E18" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="F18" t="s">
         <v>268</v>
@@ -3889,7 +3892,7 @@
         <v>45</v>
       </c>
       <c r="E19" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="F19" t="s">
         <v>269</v>
@@ -3969,7 +3972,7 @@
         <v>46</v>
       </c>
       <c r="E20" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="F20" t="s">
         <v>270</v>
@@ -4049,7 +4052,7 @@
         <v>47</v>
       </c>
       <c r="E21" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="F21" t="s">
         <v>271</v>
@@ -4129,7 +4132,7 @@
         <v>48</v>
       </c>
       <c r="E22" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="F22" t="s">
         <v>272</v>
@@ -4209,7 +4212,7 @@
         <v>49</v>
       </c>
       <c r="E23" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="F23" t="s">
         <v>273</v>
@@ -4289,7 +4292,7 @@
         <v>50</v>
       </c>
       <c r="E24" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="F24" t="s">
         <v>274</v>
@@ -4369,7 +4372,7 @@
         <v>51</v>
       </c>
       <c r="E25" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="F25" t="s">
         <v>275</v>
@@ -4449,7 +4452,7 @@
         <v>52</v>
       </c>
       <c r="E26" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="F26" t="s">
         <v>276</v>
@@ -4529,7 +4532,7 @@
         <v>53</v>
       </c>
       <c r="E27" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="F27" t="s">
         <v>277</v>
@@ -4609,7 +4612,7 @@
         <v>54</v>
       </c>
       <c r="E28" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="F28" t="s">
         <v>278</v>
@@ -4689,7 +4692,7 @@
         <v>55</v>
       </c>
       <c r="E29" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="F29" t="s">
         <v>279</v>
@@ -4769,7 +4772,7 @@
         <v>56</v>
       </c>
       <c r="E30" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="F30" t="s">
         <v>280</v>
@@ -4849,7 +4852,7 @@
         <v>57</v>
       </c>
       <c r="E31" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F31" t="s">
         <v>281</v>
@@ -4929,7 +4932,7 @@
         <v>58</v>
       </c>
       <c r="E32" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F32" t="s">
         <v>282</v>
@@ -5009,7 +5012,7 @@
         <v>59</v>
       </c>
       <c r="E33" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="F33" t="s">
         <v>283</v>
@@ -5089,7 +5092,7 @@
         <v>60</v>
       </c>
       <c r="E34" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="F34" t="s">
         <v>284</v>
@@ -5169,7 +5172,7 @@
         <v>61</v>
       </c>
       <c r="E35" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="F35" t="s">
         <v>285</v>
@@ -5249,7 +5252,7 @@
         <v>62</v>
       </c>
       <c r="E36" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="F36" t="s">
         <v>286</v>
@@ -5329,7 +5332,7 @@
         <v>63</v>
       </c>
       <c r="E37" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="F37" t="s">
         <v>287</v>
@@ -5409,7 +5412,7 @@
         <v>64</v>
       </c>
       <c r="E38" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="F38" t="s">
         <v>288</v>
@@ -5489,7 +5492,7 @@
         <v>65</v>
       </c>
       <c r="E39" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="F39" t="s">
         <v>289</v>
@@ -5569,7 +5572,7 @@
         <v>66</v>
       </c>
       <c r="E40" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="F40" t="s">
         <v>290</v>
@@ -5649,7 +5652,7 @@
         <v>67</v>
       </c>
       <c r="E41" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="F41" t="s">
         <v>291</v>
@@ -5729,7 +5732,7 @@
         <v>68</v>
       </c>
       <c r="E42" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="F42" t="s">
         <v>292</v>
@@ -5809,7 +5812,7 @@
         <v>69</v>
       </c>
       <c r="E43" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="F43" t="s">
         <v>293</v>
@@ -5889,7 +5892,7 @@
         <v>70</v>
       </c>
       <c r="E44" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="F44" t="s">
         <v>294</v>
@@ -5969,7 +5972,7 @@
         <v>71</v>
       </c>
       <c r="E45" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="F45" t="s">
         <v>295</v>
@@ -6049,7 +6052,7 @@
         <v>72</v>
       </c>
       <c r="E46" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="F46" t="s">
         <v>296</v>
@@ -6129,7 +6132,7 @@
         <v>73</v>
       </c>
       <c r="E47" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="F47" t="s">
         <v>297</v>
@@ -6209,7 +6212,7 @@
         <v>74</v>
       </c>
       <c r="E48" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="F48" t="s">
         <v>298</v>
@@ -6289,7 +6292,7 @@
         <v>75</v>
       </c>
       <c r="E49" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="F49" t="s">
         <v>299</v>
@@ -6369,7 +6372,7 @@
         <v>76</v>
       </c>
       <c r="E50" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="F50" t="s">
         <v>300</v>
@@ -6449,7 +6452,7 @@
         <v>77</v>
       </c>
       <c r="E51" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="F51" t="s">
         <v>301</v>
@@ -6529,7 +6532,7 @@
         <v>78</v>
       </c>
       <c r="E52" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="F52" t="s">
         <v>302</v>
@@ -6609,7 +6612,7 @@
         <v>79</v>
       </c>
       <c r="E53" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="F53" t="s">
         <v>303</v>
@@ -6689,7 +6692,7 @@
         <v>80</v>
       </c>
       <c r="E54" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="F54" t="s">
         <v>304</v>
@@ -6769,7 +6772,7 @@
         <v>81</v>
       </c>
       <c r="E55" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="F55" t="s">
         <v>305</v>
@@ -6849,7 +6852,7 @@
         <v>82</v>
       </c>
       <c r="E56" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="F56" t="s">
         <v>306</v>
@@ -6929,7 +6932,7 @@
         <v>83</v>
       </c>
       <c r="E57" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="F57" t="s">
         <v>307</v>
@@ -7009,7 +7012,7 @@
         <v>84</v>
       </c>
       <c r="E58" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="F58" t="s">
         <v>308</v>
@@ -7089,7 +7092,7 @@
         <v>85</v>
       </c>
       <c r="E59" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="F59" t="s">
         <v>309</v>
@@ -7169,7 +7172,7 @@
         <v>86</v>
       </c>
       <c r="E60" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="F60" t="s">
         <v>310</v>
@@ -7249,7 +7252,7 @@
         <v>87</v>
       </c>
       <c r="E61" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="F61" t="s">
         <v>311</v>
@@ -7329,7 +7332,7 @@
         <v>88</v>
       </c>
       <c r="E62" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="F62" t="s">
         <v>312</v>
@@ -7409,7 +7412,7 @@
         <v>89</v>
       </c>
       <c r="E63" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="F63" t="s">
         <v>313</v>
@@ -7489,7 +7492,7 @@
         <v>90</v>
       </c>
       <c r="E64" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="F64" t="s">
         <v>314</v>
@@ -7569,7 +7572,7 @@
         <v>91</v>
       </c>
       <c r="E65" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="F65" t="s">
         <v>315</v>
@@ -7649,7 +7652,7 @@
         <v>92</v>
       </c>
       <c r="E66" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="F66" t="s">
         <v>316</v>
@@ -7729,7 +7732,7 @@
         <v>93</v>
       </c>
       <c r="E67" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="F67" t="s">
         <v>317</v>
@@ -7809,7 +7812,7 @@
         <v>94</v>
       </c>
       <c r="E68" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="F68" t="s">
         <v>318</v>
@@ -7889,7 +7892,7 @@
         <v>95</v>
       </c>
       <c r="E69" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="F69" t="s">
         <v>319</v>
@@ -7969,7 +7972,7 @@
         <v>96</v>
       </c>
       <c r="E70" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="F70" t="s">
         <v>320</v>
@@ -8049,7 +8052,7 @@
         <v>97</v>
       </c>
       <c r="E71" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="F71" t="s">
         <v>321</v>
@@ -8129,7 +8132,7 @@
         <v>98</v>
       </c>
       <c r="E72" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="F72" t="s">
         <v>322</v>
@@ -8209,7 +8212,7 @@
         <v>99</v>
       </c>
       <c r="E73" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="F73" t="s">
         <v>323</v>
@@ -8289,7 +8292,7 @@
         <v>100</v>
       </c>
       <c r="E74" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="F74" t="s">
         <v>324</v>
@@ -8369,7 +8372,7 @@
         <v>101</v>
       </c>
       <c r="E75" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F75" t="s">
         <v>325</v>
@@ -8449,7 +8452,7 @@
         <v>102</v>
       </c>
       <c r="E76" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="F76" t="s">
         <v>326</v>
@@ -8529,7 +8532,7 @@
         <v>103</v>
       </c>
       <c r="E77" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="F77" t="s">
         <v>327</v>
@@ -8609,7 +8612,7 @@
         <v>104</v>
       </c>
       <c r="E78" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="F78" t="s">
         <v>328</v>
@@ -8689,7 +8692,7 @@
         <v>105</v>
       </c>
       <c r="E79" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="F79" t="s">
         <v>329</v>
@@ -8769,7 +8772,7 @@
         <v>106</v>
       </c>
       <c r="E80" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="F80" t="s">
         <v>330</v>
@@ -8849,7 +8852,7 @@
         <v>107</v>
       </c>
       <c r="E81" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="F81" t="s">
         <v>331</v>
@@ -8929,7 +8932,7 @@
         <v>108</v>
       </c>
       <c r="E82" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="F82" t="s">
         <v>332</v>
@@ -9009,7 +9012,7 @@
         <v>109</v>
       </c>
       <c r="E83" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="F83" t="s">
         <v>333</v>
@@ -9089,7 +9092,7 @@
         <v>110</v>
       </c>
       <c r="E84" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="F84" t="s">
         <v>334</v>
@@ -9169,7 +9172,7 @@
         <v>111</v>
       </c>
       <c r="E85" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="F85" t="s">
         <v>335</v>
@@ -9249,7 +9252,7 @@
         <v>112</v>
       </c>
       <c r="E86" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="F86" t="s">
         <v>336</v>
@@ -9329,7 +9332,7 @@
         <v>113</v>
       </c>
       <c r="E87" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="F87" t="s">
         <v>337</v>
@@ -9409,7 +9412,7 @@
         <v>114</v>
       </c>
       <c r="E88" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="F88" t="s">
         <v>338</v>
@@ -9489,7 +9492,7 @@
         <v>115</v>
       </c>
       <c r="E89" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="F89" t="s">
         <v>339</v>
@@ -9569,7 +9572,7 @@
         <v>116</v>
       </c>
       <c r="E90" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="F90" t="s">
         <v>340</v>
@@ -9649,7 +9652,7 @@
         <v>117</v>
       </c>
       <c r="E91" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="F91" t="s">
         <v>341</v>
@@ -9729,7 +9732,7 @@
         <v>118</v>
       </c>
       <c r="E92" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="F92" t="s">
         <v>342</v>
@@ -9809,7 +9812,7 @@
         <v>119</v>
       </c>
       <c r="E93" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="F93" t="s">
         <v>343</v>
@@ -9889,7 +9892,7 @@
         <v>120</v>
       </c>
       <c r="E94" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="F94" t="s">
         <v>344</v>
@@ -9969,7 +9972,7 @@
         <v>121</v>
       </c>
       <c r="E95" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="F95" t="s">
         <v>345</v>
@@ -10049,7 +10052,7 @@
         <v>122</v>
       </c>
       <c r="E96" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="F96" t="s">
         <v>346</v>
@@ -10129,7 +10132,7 @@
         <v>123</v>
       </c>
       <c r="E97" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="F97" t="s">
         <v>347</v>
@@ -10209,7 +10212,7 @@
         <v>124</v>
       </c>
       <c r="E98" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F98" t="s">
         <v>348</v>
@@ -10289,7 +10292,7 @@
         <v>125</v>
       </c>
       <c r="E99" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="F99" t="s">
         <v>349</v>
@@ -10369,7 +10372,7 @@
         <v>126</v>
       </c>
       <c r="E100" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="F100" t="s">
         <v>350</v>
@@ -10449,7 +10452,7 @@
         <v>127</v>
       </c>
       <c r="E101" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="F101" t="s">
         <v>351</v>
@@ -10529,7 +10532,7 @@
         <v>128</v>
       </c>
       <c r="E102" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="F102" t="s">
         <v>352</v>
@@ -10609,7 +10612,7 @@
         <v>129</v>
       </c>
       <c r="E103" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="F103" t="s">
         <v>353</v>
@@ -10689,7 +10692,7 @@
         <v>130</v>
       </c>
       <c r="E104" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="F104" t="s">
         <v>354</v>
@@ -10769,7 +10772,7 @@
         <v>131</v>
       </c>
       <c r="E105" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="F105" t="s">
         <v>355</v>
@@ -10849,7 +10852,7 @@
         <v>132</v>
       </c>
       <c r="E106" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="F106" t="s">
         <v>8</v>
@@ -10929,7 +10932,7 @@
         <v>133</v>
       </c>
       <c r="E107" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="F107" t="s">
         <v>356</v>
@@ -11009,7 +11012,7 @@
         <v>134</v>
       </c>
       <c r="E108" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="F108" t="s">
         <v>357</v>
@@ -11089,7 +11092,7 @@
         <v>135</v>
       </c>
       <c r="E109" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="F109" t="s">
         <v>358</v>
@@ -11169,7 +11172,7 @@
         <v>136</v>
       </c>
       <c r="E110" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="F110" t="s">
         <v>359</v>
@@ -11249,7 +11252,7 @@
         <v>137</v>
       </c>
       <c r="E111" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="F111" t="s">
         <v>360</v>
@@ -11329,7 +11332,7 @@
         <v>138</v>
       </c>
       <c r="E112" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="F112" t="s">
         <v>361</v>
@@ -11409,7 +11412,7 @@
         <v>139</v>
       </c>
       <c r="E113" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="F113" t="s">
         <v>362</v>
@@ -11489,7 +11492,7 @@
         <v>140</v>
       </c>
       <c r="E114" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="F114" t="s">
         <v>363</v>
@@ -11569,7 +11572,7 @@
         <v>141</v>
       </c>
       <c r="E115" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="F115" t="s">
         <v>364</v>
@@ -11649,7 +11652,7 @@
         <v>142</v>
       </c>
       <c r="E116" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="F116" t="s">
         <v>365</v>
@@ -11729,7 +11732,7 @@
         <v>143</v>
       </c>
       <c r="E117" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="F117" t="s">
         <v>366</v>
@@ -11809,7 +11812,7 @@
         <v>144</v>
       </c>
       <c r="E118" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="F118" t="s">
         <v>367</v>
@@ -11889,7 +11892,7 @@
         <v>145</v>
       </c>
       <c r="E119" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="F119" t="s">
         <v>368</v>
@@ -11969,7 +11972,7 @@
         <v>146</v>
       </c>
       <c r="E120" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="F120" t="s">
         <v>369</v>
@@ -12049,7 +12052,7 @@
         <v>147</v>
       </c>
       <c r="E121" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="F121" t="s">
         <v>370</v>
@@ -12129,7 +12132,7 @@
         <v>148</v>
       </c>
       <c r="E122" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="F122" t="s">
         <v>371</v>
@@ -12209,7 +12212,7 @@
         <v>149</v>
       </c>
       <c r="E123" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="F123" t="s">
         <v>372</v>
@@ -12289,7 +12292,7 @@
         <v>150</v>
       </c>
       <c r="E124" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="F124" t="s">
         <v>373</v>
@@ -12369,7 +12372,7 @@
         <v>151</v>
       </c>
       <c r="E125" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="F125" t="s">
         <v>374</v>
@@ -12449,7 +12452,7 @@
         <v>152</v>
       </c>
       <c r="E126" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="F126" t="s">
         <v>375</v>
@@ -12529,7 +12532,7 @@
         <v>153</v>
       </c>
       <c r="E127" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="F127" t="s">
         <v>376</v>
@@ -12609,7 +12612,7 @@
         <v>154</v>
       </c>
       <c r="E128" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="F128" t="s">
         <v>377</v>
@@ -12689,7 +12692,7 @@
         <v>155</v>
       </c>
       <c r="E129" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="F129" t="s">
         <v>378</v>
@@ -12769,7 +12772,7 @@
         <v>156</v>
       </c>
       <c r="E130" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="F130" t="s">
         <v>379</v>
@@ -12849,7 +12852,7 @@
         <v>157</v>
       </c>
       <c r="E131" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="F131" t="s">
         <v>380</v>
@@ -12929,7 +12932,7 @@
         <v>158</v>
       </c>
       <c r="E132" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="F132" t="s">
         <v>381</v>
@@ -13009,7 +13012,7 @@
         <v>159</v>
       </c>
       <c r="E133" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="F133" t="s">
         <v>382</v>
@@ -13089,7 +13092,7 @@
         <v>160</v>
       </c>
       <c r="E134" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="F134" t="s">
         <v>383</v>
@@ -13169,7 +13172,7 @@
         <v>161</v>
       </c>
       <c r="E135" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="F135" t="s">
         <v>384</v>
@@ -13249,7 +13252,7 @@
         <v>162</v>
       </c>
       <c r="E136" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="F136" t="s">
         <v>385</v>
@@ -13329,7 +13332,7 @@
         <v>163</v>
       </c>
       <c r="E137" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="F137" t="s">
         <v>386</v>
@@ -13409,7 +13412,7 @@
         <v>164</v>
       </c>
       <c r="E138" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="F138" t="s">
         <v>387</v>
@@ -13489,7 +13492,7 @@
         <v>165</v>
       </c>
       <c r="E139" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="F139" t="s">
         <v>388</v>
@@ -13569,7 +13572,7 @@
         <v>166</v>
       </c>
       <c r="E140" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="F140" t="s">
         <v>389</v>
@@ -13649,7 +13652,7 @@
         <v>167</v>
       </c>
       <c r="E141" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="F141" t="s">
         <v>390</v>
@@ -13729,7 +13732,7 @@
         <v>168</v>
       </c>
       <c r="E142" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="F142" t="s">
         <v>391</v>
@@ -13809,7 +13812,7 @@
         <v>169</v>
       </c>
       <c r="E143" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="F143" t="s">
         <v>392</v>
@@ -13889,7 +13892,7 @@
         <v>170</v>
       </c>
       <c r="E144" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="F144" t="s">
         <v>393</v>
@@ -13969,7 +13972,7 @@
         <v>171</v>
       </c>
       <c r="E145" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="F145" t="s">
         <v>394</v>
@@ -14049,7 +14052,7 @@
         <v>172</v>
       </c>
       <c r="E146" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="F146" t="s">
         <v>395</v>
@@ -14129,7 +14132,7 @@
         <v>173</v>
       </c>
       <c r="E147" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="F147" t="s">
         <v>396</v>
@@ -14209,7 +14212,7 @@
         <v>174</v>
       </c>
       <c r="E148" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="F148" t="s">
         <v>397</v>
@@ -14289,7 +14292,7 @@
         <v>175</v>
       </c>
       <c r="E149" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="F149" t="s">
         <v>398</v>
@@ -14369,7 +14372,7 @@
         <v>176</v>
       </c>
       <c r="E150" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="F150" t="s">
         <v>399</v>
@@ -14449,7 +14452,7 @@
         <v>177</v>
       </c>
       <c r="E151" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="F151" t="s">
         <v>400</v>
@@ -14529,7 +14532,7 @@
         <v>178</v>
       </c>
       <c r="E152" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="F152" t="s">
         <v>401</v>
@@ -14609,7 +14612,7 @@
         <v>179</v>
       </c>
       <c r="E153" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="F153" t="s">
         <v>402</v>
@@ -14689,7 +14692,7 @@
         <v>180</v>
       </c>
       <c r="E154" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="F154" t="s">
         <v>403</v>
@@ -14769,7 +14772,7 @@
         <v>181</v>
       </c>
       <c r="E155" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="F155" t="s">
         <v>404</v>
@@ -14849,7 +14852,7 @@
         <v>182</v>
       </c>
       <c r="E156" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="F156" t="s">
         <v>405</v>
@@ -14929,7 +14932,7 @@
         <v>183</v>
       </c>
       <c r="E157" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="F157" t="s">
         <v>406</v>
@@ -15009,7 +15012,7 @@
         <v>184</v>
       </c>
       <c r="E158" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="F158" t="s">
         <v>407</v>
@@ -15089,7 +15092,7 @@
         <v>185</v>
       </c>
       <c r="E159" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="F159" t="s">
         <v>408</v>
@@ -15169,7 +15172,7 @@
         <v>186</v>
       </c>
       <c r="E160" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="F160" t="s">
         <v>409</v>
@@ -15249,7 +15252,7 @@
         <v>187</v>
       </c>
       <c r="E161" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="F161" t="s">
         <v>410</v>
@@ -15329,7 +15332,7 @@
         <v>188</v>
       </c>
       <c r="E162" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="F162" t="s">
         <v>411</v>
@@ -15409,7 +15412,7 @@
         <v>189</v>
       </c>
       <c r="E163" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="F163" t="s">
         <v>412</v>
@@ -15489,7 +15492,7 @@
         <v>190</v>
       </c>
       <c r="E164" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="F164" t="s">
         <v>413</v>
@@ -15569,7 +15572,7 @@
         <v>191</v>
       </c>
       <c r="E165" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="F165" t="s">
         <v>414</v>
@@ -15649,7 +15652,7 @@
         <v>192</v>
       </c>
       <c r="E166" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="F166" t="s">
         <v>415</v>
@@ -15729,7 +15732,7 @@
         <v>193</v>
       </c>
       <c r="E167" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="F167" t="s">
         <v>416</v>
@@ -15809,7 +15812,7 @@
         <v>194</v>
       </c>
       <c r="E168" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="F168" t="s">
         <v>417</v>
@@ -15889,7 +15892,7 @@
         <v>195</v>
       </c>
       <c r="E169" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="F169" t="s">
         <v>418</v>
@@ -15969,7 +15972,7 @@
         <v>196</v>
       </c>
       <c r="E170" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="F170" t="s">
         <v>419</v>
@@ -16049,7 +16052,7 @@
         <v>197</v>
       </c>
       <c r="E171" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="F171" t="s">
         <v>420</v>
@@ -16129,7 +16132,7 @@
         <v>198</v>
       </c>
       <c r="E172" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="F172" t="s">
         <v>421</v>
@@ -16209,7 +16212,7 @@
         <v>199</v>
       </c>
       <c r="E173" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="F173" t="s">
         <v>422</v>
@@ -16289,7 +16292,7 @@
         <v>200</v>
       </c>
       <c r="E174" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="F174" t="s">
         <v>423</v>
@@ -16369,7 +16372,7 @@
         <v>201</v>
       </c>
       <c r="E175" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="F175" t="s">
         <v>424</v>
@@ -16449,7 +16452,7 @@
         <v>202</v>
       </c>
       <c r="E176" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="F176" t="s">
         <v>425</v>
@@ -16529,7 +16532,7 @@
         <v>203</v>
       </c>
       <c r="E177" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="F177" t="s">
         <v>426</v>
@@ -16609,7 +16612,7 @@
         <v>204</v>
       </c>
       <c r="E178" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="F178" t="s">
         <v>427</v>
@@ -16689,7 +16692,7 @@
         <v>205</v>
       </c>
       <c r="E179" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="F179" t="s">
         <v>428</v>
@@ -16769,7 +16772,7 @@
         <v>206</v>
       </c>
       <c r="E180" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="F180" t="s">
         <v>429</v>
@@ -16849,7 +16852,7 @@
         <v>207</v>
       </c>
       <c r="E181" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="F181" t="s">
         <v>430</v>
@@ -16929,7 +16932,7 @@
         <v>208</v>
       </c>
       <c r="E182" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="F182" t="s">
         <v>431</v>
@@ -17009,7 +17012,7 @@
         <v>209</v>
       </c>
       <c r="E183" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="F183" t="s">
         <v>432</v>
@@ -17089,7 +17092,7 @@
         <v>210</v>
       </c>
       <c r="E184" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="F184" t="s">
         <v>433</v>
@@ -17166,10 +17169,10 @@
         <v>434</v>
       </c>
       <c r="D185" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="E185" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="F185" t="s">
         <v>434</v>
@@ -17249,7 +17252,7 @@
         <v>212</v>
       </c>
       <c r="E186" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="F186" t="s">
         <v>435</v>
@@ -17329,7 +17332,7 @@
         <v>213</v>
       </c>
       <c r="E187" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="F187" t="s">
         <v>436</v>
@@ -17409,7 +17412,7 @@
         <v>214</v>
       </c>
       <c r="E188" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="F188" t="s">
         <v>437</v>
@@ -17489,7 +17492,7 @@
         <v>215</v>
       </c>
       <c r="E189" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="F189" t="s">
         <v>438</v>
@@ -17569,7 +17572,7 @@
         <v>216</v>
       </c>
       <c r="E190" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="F190" t="s">
         <v>439</v>
@@ -17649,7 +17652,7 @@
         <v>217</v>
       </c>
       <c r="E191" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="F191" t="s">
         <v>440</v>
@@ -17729,7 +17732,7 @@
         <v>218</v>
       </c>
       <c r="E192" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="F192" t="s">
         <v>441</v>
@@ -17809,7 +17812,7 @@
         <v>219</v>
       </c>
       <c r="E193" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="F193" t="s">
         <v>442</v>
@@ -17889,7 +17892,7 @@
         <v>220</v>
       </c>
       <c r="E194" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="F194" t="s">
         <v>443</v>
@@ -17969,7 +17972,7 @@
         <v>221</v>
       </c>
       <c r="E195" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="F195" t="s">
         <v>444</v>
@@ -18049,7 +18052,7 @@
         <v>222</v>
       </c>
       <c r="E196" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="F196" t="s">
         <v>445</v>
@@ -18129,7 +18132,7 @@
         <v>223</v>
       </c>
       <c r="E197" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="F197" t="s">
         <v>446</v>
@@ -18209,7 +18212,7 @@
         <v>224</v>
       </c>
       <c r="E198" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="F198" t="s">
         <v>447</v>
@@ -18289,7 +18292,7 @@
         <v>225</v>
       </c>
       <c r="E199" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="F199" t="s">
         <v>448</v>
@@ -18369,7 +18372,7 @@
         <v>226</v>
       </c>
       <c r="E200" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="F200" t="s">
         <v>449</v>
@@ -18449,7 +18452,7 @@
         <v>227</v>
       </c>
       <c r="E201" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="F201" t="s">
         <v>450</v>
@@ -18529,7 +18532,7 @@
         <v>228</v>
       </c>
       <c r="E202" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="F202" t="s">
         <v>451</v>
@@ -18609,7 +18612,7 @@
         <v>229</v>
       </c>
       <c r="E203" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="F203" t="s">
         <v>452</v>
@@ -18689,7 +18692,7 @@
         <v>230</v>
       </c>
       <c r="E204" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="F204" t="s">
         <v>453</v>
@@ -18769,7 +18772,7 @@
         <v>231</v>
       </c>
       <c r="E205" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="F205" t="s">
         <v>454</v>
@@ -18849,7 +18852,7 @@
         <v>232</v>
       </c>
       <c r="E206" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="F206" t="s">
         <v>455</v>
@@ -18929,7 +18932,7 @@
         <v>233</v>
       </c>
       <c r="E207" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="F207" t="s">
         <v>456</v>
@@ -19009,7 +19012,7 @@
         <v>234</v>
       </c>
       <c r="E208" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="F208" t="s">
         <v>457</v>
@@ -19089,7 +19092,7 @@
         <v>235</v>
       </c>
       <c r="E209" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="F209" t="s">
         <v>458</v>
@@ -19169,7 +19172,7 @@
         <v>236</v>
       </c>
       <c r="E210" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="F210" t="s">
         <v>459</v>
@@ -19249,7 +19252,7 @@
         <v>237</v>
       </c>
       <c r="E211" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="F211" t="s">
         <v>460</v>
@@ -19329,7 +19332,7 @@
         <v>238</v>
       </c>
       <c r="E212" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="F212" t="s">
         <v>461</v>
@@ -19409,7 +19412,7 @@
         <v>239</v>
       </c>
       <c r="E213" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="F213" t="s">
         <v>462</v>
@@ -19489,7 +19492,7 @@
         <v>240</v>
       </c>
       <c r="E214" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="F214" t="s">
         <v>463</v>
@@ -19569,7 +19572,7 @@
         <v>241</v>
       </c>
       <c r="E215" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="F215" t="s">
         <v>464</v>
@@ -19649,7 +19652,7 @@
         <v>242</v>
       </c>
       <c r="E216" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="F216" t="s">
         <v>465</v>
@@ -19729,7 +19732,7 @@
         <v>243</v>
       </c>
       <c r="E217" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="F217" t="s">
         <v>466</v>
@@ -19809,7 +19812,7 @@
         <v>244</v>
       </c>
       <c r="E218" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="F218" t="s">
         <v>467</v>
@@ -19889,7 +19892,7 @@
         <v>245</v>
       </c>
       <c r="E219" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="F219" t="s">
         <v>468</v>
@@ -19966,10 +19969,10 @@
         <v>469</v>
       </c>
       <c r="D220" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="E220" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="F220" t="s">
         <v>434</v>
@@ -20049,7 +20052,7 @@
         <v>37</v>
       </c>
       <c r="E221" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="F221" t="s">
         <v>261</v>
@@ -20129,7 +20132,7 @@
         <v>108</v>
       </c>
       <c r="E222" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="F222" t="s">
         <v>332</v>
@@ -20209,7 +20212,7 @@
         <v>82</v>
       </c>
       <c r="E223" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="F223" t="s">
         <v>306</v>
@@ -20289,7 +20292,7 @@
         <v>116</v>
       </c>
       <c r="E224" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="F224" t="s">
         <v>340</v>
@@ -20369,7 +20372,7 @@
         <v>127</v>
       </c>
       <c r="E225" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="F225" t="s">
         <v>351</v>
@@ -20449,7 +20452,7 @@
         <v>128</v>
       </c>
       <c r="E226" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="F226" t="s">
         <v>352</v>
@@ -20529,7 +20532,7 @@
         <v>104</v>
       </c>
       <c r="E227" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="F227" t="s">
         <v>328</v>
@@ -20609,7 +20612,7 @@
         <v>88</v>
       </c>
       <c r="E228" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="F228" t="s">
         <v>312</v>
@@ -20689,7 +20692,7 @@
         <v>113</v>
       </c>
       <c r="E229" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="F229" t="s">
         <v>337</v>
@@ -20769,7 +20772,7 @@
         <v>132</v>
       </c>
       <c r="E230" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="F230" t="s">
         <v>8</v>
@@ -20839,630 +20842,81 @@
       <c r="A231" t="s">
         <v>247</v>
       </c>
-      <c r="B231" t="s">
-        <v>251</v>
-      </c>
       <c r="C231" t="s">
-        <v>469</v>
-      </c>
-      <c r="D231" t="s">
         <v>470</v>
-      </c>
-      <c r="E231" t="s">
-        <v>649</v>
-      </c>
-      <c r="F231" t="s">
-        <v>434</v>
-      </c>
-      <c r="G231">
-        <v>50</v>
-      </c>
-      <c r="H231">
-        <v>186</v>
-      </c>
-      <c r="I231">
-        <v>26.1</v>
-      </c>
-      <c r="J231">
-        <v>6.95</v>
-      </c>
-      <c r="K231">
-        <v>16.655</v>
-      </c>
-      <c r="L231">
-        <v>0</v>
-      </c>
-      <c r="M231">
-        <v>0</v>
-      </c>
-      <c r="N231">
-        <v>4</v>
-      </c>
-      <c r="O231">
-        <v>0.245</v>
-      </c>
-      <c r="P231">
-        <v>0.9</v>
-      </c>
-      <c r="Q231">
-        <v>9</v>
-      </c>
-      <c r="R231">
-        <v>0.2395</v>
-      </c>
-      <c r="S231">
-        <v>0.0815</v>
-      </c>
-      <c r="T231">
-        <v>0.8685</v>
-      </c>
-      <c r="U231">
-        <v>0</v>
-      </c>
-      <c r="V231">
-        <v>0.5</v>
-      </c>
-      <c r="W231">
-        <v>0.26</v>
-      </c>
-      <c r="X231">
-        <v>0.295</v>
-      </c>
-      <c r="Y231">
-        <v>0.355</v>
-      </c>
-      <c r="Z231">
-        <v>56</v>
       </c>
     </row>
     <row r="232" spans="1:26">
       <c r="A232" t="s">
         <v>247</v>
       </c>
-      <c r="B232" t="s">
-        <v>251</v>
-      </c>
       <c r="C232" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="D232" t="s">
-        <v>37</v>
-      </c>
-      <c r="E232" t="s">
-        <v>480</v>
+        <v>104</v>
       </c>
       <c r="F232" t="s">
-        <v>261</v>
+        <v>328</v>
       </c>
       <c r="G232">
-        <v>6.66</v>
+        <v>100</v>
       </c>
       <c r="H232">
-        <v>94</v>
+        <v>900</v>
       </c>
       <c r="I232">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="J232">
-        <v>4.05</v>
+        <v>0</v>
       </c>
       <c r="K232">
-        <v>0.3</v>
+        <v>100</v>
       </c>
       <c r="L232">
-        <v>13.4</v>
+        <v>0</v>
       </c>
       <c r="M232">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="N232">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="O232">
-        <v>1.1</v>
+        <v>0.05</v>
       </c>
       <c r="P232">
-        <v>0.9</v>
+        <v>0.67</v>
       </c>
       <c r="Q232">
         <v>0</v>
       </c>
       <c r="R232">
-        <v>0.24</v>
+        <v>0</v>
       </c>
       <c r="S232">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="T232">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="U232">
-        <v>1.2</v>
+        <v>0.033</v>
       </c>
       <c r="V232">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W232">
         <v>0</v>
       </c>
       <c r="X232">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="Y232">
         <v>0</v>
       </c>
       <c r="Z232">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="233" spans="1:26">
-      <c r="A233" t="s">
-        <v>247</v>
-      </c>
-      <c r="B233" t="s">
-        <v>251</v>
-      </c>
-      <c r="C233" t="s">
-        <v>469</v>
-      </c>
-      <c r="D233" t="s">
-        <v>108</v>
-      </c>
-      <c r="E233" t="s">
-        <v>551</v>
-      </c>
-      <c r="F233" t="s">
-        <v>332</v>
-      </c>
-      <c r="G233">
-        <v>3.33</v>
-      </c>
-      <c r="H233">
-        <v>0</v>
-      </c>
-      <c r="I233">
-        <v>1</v>
-      </c>
-      <c r="J233">
-        <v>0</v>
-      </c>
-      <c r="K233">
-        <v>0</v>
-      </c>
-      <c r="L233">
-        <v>0</v>
-      </c>
-      <c r="M233">
-        <v>0</v>
-      </c>
-      <c r="N233">
-        <v>150</v>
-      </c>
-      <c r="O233">
-        <v>0.8</v>
-      </c>
-      <c r="P233">
-        <v>0</v>
-      </c>
-      <c r="Q233">
-        <v>0</v>
-      </c>
-      <c r="R233">
-        <v>0</v>
-      </c>
-      <c r="S233">
-        <v>0</v>
-      </c>
-      <c r="T233">
-        <v>0</v>
-      </c>
-      <c r="U233">
-        <v>0</v>
-      </c>
-      <c r="V233">
-        <v>0</v>
-      </c>
-      <c r="W233">
-        <v>0</v>
-      </c>
-      <c r="X233">
-        <v>0</v>
-      </c>
-      <c r="Y233">
-        <v>0</v>
-      </c>
-      <c r="Z233">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="234" spans="1:26">
-      <c r="A234" t="s">
-        <v>247</v>
-      </c>
-      <c r="B234" t="s">
-        <v>251</v>
-      </c>
-      <c r="C234" t="s">
-        <v>469</v>
-      </c>
-      <c r="D234" t="s">
-        <v>82</v>
-      </c>
-      <c r="E234" t="s">
-        <v>525</v>
-      </c>
-      <c r="F234" t="s">
-        <v>306</v>
-      </c>
-      <c r="G234">
-        <v>10</v>
-      </c>
-      <c r="H234">
-        <v>375</v>
-      </c>
-      <c r="I234">
-        <v>5.5</v>
-      </c>
-      <c r="J234">
-        <v>0.7</v>
-      </c>
-      <c r="K234">
-        <v>0.25</v>
-      </c>
-      <c r="L234">
-        <v>92.5</v>
-      </c>
-      <c r="M234">
-        <v>0.2</v>
-      </c>
-      <c r="N234">
-        <v>168</v>
-      </c>
-      <c r="O234">
-        <v>1.55</v>
-      </c>
-      <c r="P234">
-        <v>0.33</v>
-      </c>
-      <c r="Q234">
-        <v>0</v>
-      </c>
-      <c r="R234">
-        <v>0.04</v>
-      </c>
-      <c r="S234">
-        <v>0.03</v>
-      </c>
-      <c r="T234">
-        <v>0.5</v>
-      </c>
-      <c r="U234">
-        <v>0.04</v>
-      </c>
-      <c r="V234">
-        <v>1</v>
-      </c>
-      <c r="W234">
-        <v>0</v>
-      </c>
-      <c r="X234">
-        <v>0</v>
-      </c>
-      <c r="Y234">
-        <v>0</v>
-      </c>
-      <c r="Z234">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="235" spans="1:26">
-      <c r="A235" t="s">
-        <v>247</v>
-      </c>
-      <c r="B235" t="s">
-        <v>251</v>
-      </c>
-      <c r="C235" t="s">
-        <v>469</v>
-      </c>
-      <c r="D235" t="s">
-        <v>116</v>
-      </c>
-      <c r="E235" t="s">
-        <v>559</v>
-      </c>
-      <c r="F235" t="s">
-        <v>340</v>
-      </c>
-      <c r="G235">
-        <v>1.66</v>
-      </c>
-      <c r="H235">
-        <v>314</v>
-      </c>
-      <c r="I235">
-        <v>13.3</v>
-      </c>
-      <c r="J235">
-        <v>9.699999999999999</v>
-      </c>
-      <c r="K235">
-        <v>7.35</v>
-      </c>
-      <c r="L235">
-        <v>39.6</v>
-      </c>
-      <c r="M235">
-        <v>25.3</v>
-      </c>
-      <c r="N235">
-        <v>497</v>
-      </c>
-      <c r="O235">
-        <v>6.6</v>
-      </c>
-      <c r="P235">
-        <v>0.3</v>
-      </c>
-      <c r="Q235">
-        <v>13</v>
-      </c>
-      <c r="R235">
-        <v>0.045</v>
-      </c>
-      <c r="S235">
-        <v>0.14</v>
-      </c>
-      <c r="T235">
-        <v>2.6</v>
-      </c>
-      <c r="U235">
-        <v>0.29</v>
-      </c>
-      <c r="V235">
-        <v>10</v>
-      </c>
-      <c r="W235">
-        <v>0</v>
-      </c>
-      <c r="X235">
-        <v>1.5</v>
-      </c>
-      <c r="Y235">
-        <v>0</v>
-      </c>
-      <c r="Z235">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="236" spans="1:26">
-      <c r="A236" t="s">
-        <v>247</v>
-      </c>
-      <c r="B236" t="s">
-        <v>251</v>
-      </c>
-      <c r="C236" t="s">
-        <v>469</v>
-      </c>
-      <c r="D236" t="s">
-        <v>127</v>
-      </c>
-      <c r="E236" t="s">
-        <v>569</v>
-      </c>
-      <c r="F236" t="s">
-        <v>351</v>
-      </c>
-      <c r="G236">
-        <v>0.33</v>
-      </c>
-      <c r="H236">
-        <v>277</v>
-      </c>
-      <c r="I236">
-        <v>4.1</v>
-      </c>
-      <c r="J236">
-        <v>50.24</v>
-      </c>
-      <c r="K236">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="L236">
-        <v>18.9</v>
-      </c>
-      <c r="M236">
-        <v>0</v>
-      </c>
-      <c r="N236">
-        <v>6</v>
-      </c>
-      <c r="O236">
-        <v>0.34</v>
-      </c>
-      <c r="P236">
-        <v>0.74</v>
-      </c>
-      <c r="Q236">
-        <v>0</v>
-      </c>
-      <c r="R236">
-        <v>0</v>
-      </c>
-      <c r="S236">
-        <v>0</v>
-      </c>
-      <c r="T236">
-        <v>0</v>
-      </c>
-      <c r="U236">
-        <v>0</v>
-      </c>
-      <c r="V236">
-        <v>0</v>
-      </c>
-      <c r="W236">
-        <v>0</v>
-      </c>
-      <c r="X236">
-        <v>0</v>
-      </c>
-      <c r="Y236">
-        <v>0</v>
-      </c>
-      <c r="Z236">
-        <v>12682</v>
-      </c>
-    </row>
-    <row r="237" spans="1:26">
-      <c r="A237" t="s">
-        <v>247</v>
-      </c>
-      <c r="B237" t="s">
-        <v>251</v>
-      </c>
-      <c r="C237" t="s">
-        <v>469</v>
-      </c>
-      <c r="D237" t="s">
-        <v>128</v>
-      </c>
-      <c r="E237" t="s">
-        <v>570</v>
-      </c>
-      <c r="F237" t="s">
-        <v>352</v>
-      </c>
-      <c r="G237">
-        <v>5</v>
-      </c>
-      <c r="H237">
-        <v>117</v>
-      </c>
-      <c r="I237">
-        <v>58.3</v>
-      </c>
-      <c r="J237">
-        <v>2.07</v>
-      </c>
-      <c r="K237">
-        <v>0.05</v>
-      </c>
-      <c r="L237">
-        <v>27.14</v>
-      </c>
-      <c r="M237">
-        <v>0.2</v>
-      </c>
-      <c r="N237">
-        <v>12</v>
-      </c>
-      <c r="O237">
-        <v>0.26</v>
-      </c>
-      <c r="P237">
-        <v>0.79</v>
-      </c>
-      <c r="Q237">
-        <v>1</v>
-      </c>
-      <c r="R237">
-        <v>0.008999999999999999</v>
-      </c>
-      <c r="S237">
-        <v>0.013</v>
-      </c>
-      <c r="T237">
-        <v>0.952</v>
-      </c>
-      <c r="U237">
-        <v>0.011</v>
-      </c>
-      <c r="V237">
-        <v>0</v>
-      </c>
-      <c r="W237">
-        <v>0</v>
-      </c>
-      <c r="X237">
-        <v>0</v>
-      </c>
-      <c r="Y237">
-        <v>0</v>
-      </c>
-      <c r="Z237">
-        <v>4608</v>
-      </c>
-    </row>
-    <row r="238" spans="1:26">
-      <c r="A238" t="s">
-        <v>247</v>
-      </c>
-      <c r="D238" t="s">
-        <v>104</v>
-      </c>
-      <c r="F238" t="s">
-        <v>328</v>
-      </c>
-      <c r="G238">
-        <v>100</v>
-      </c>
-      <c r="H238">
-        <v>900</v>
-      </c>
-      <c r="I238">
-        <v>0</v>
-      </c>
-      <c r="J238">
-        <v>0</v>
-      </c>
-      <c r="K238">
-        <v>100</v>
-      </c>
-      <c r="L238">
-        <v>0</v>
-      </c>
-      <c r="M238">
-        <v>0</v>
-      </c>
-      <c r="N238">
-        <v>0</v>
-      </c>
-      <c r="O238">
-        <v>0.05</v>
-      </c>
-      <c r="P238">
-        <v>0.67</v>
-      </c>
-      <c r="Q238">
-        <v>0</v>
-      </c>
-      <c r="R238">
-        <v>0</v>
-      </c>
-      <c r="S238">
-        <v>0</v>
-      </c>
-      <c r="T238">
-        <v>0</v>
-      </c>
-      <c r="U238">
-        <v>0.033</v>
-      </c>
-      <c r="V238">
-        <v>0</v>
-      </c>
-      <c r="W238">
-        <v>0</v>
-      </c>
-      <c r="X238">
-        <v>0</v>
-      </c>
-      <c r="Y238">
-        <v>0</v>
-      </c>
-      <c r="Z238">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
food, ingredient DB css 수정 완료
</commit_message>
<xml_diff>
--- a/data/FoodData.xlsx
+++ b/data/FoodData.xlsx
@@ -1406,7 +1406,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Garlic, fresh, raw </t>
+          <t>Garlic, fresh, raw</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1421,7 +1421,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Garlic, fresh, raw </t>
+          <t>Garlic, fresh, raw</t>
         </is>
       </c>
       <c r="G11" t="n">
@@ -20741,7 +20741,7 @@
       </c>
       <c r="F221" t="inlineStr">
         <is>
-          <t xml:space="preserve">Garlic, fresh, raw </t>
+          <t>Garlic, fresh, raw</t>
         </is>
       </c>
       <c r="G221" t="n">

</xml_diff>